<commit_message>
working on assignment2 report.
</commit_message>
<xml_diff>
--- a/Assignment2/Report/Assignment_2_result_plot_Kazumi_v2.xlsx
+++ b/Assignment2/Report/Assignment_2_result_plot_Kazumi_v2.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KAZUMI\repo\cse436\Assignment2\Report\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5916" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17260" windowHeight="5920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="performance" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="47">
   <si>
     <t>omp_parallel 1 thread</t>
   </si>
@@ -163,12 +158,15 @@
   <si>
     <t>Thread</t>
   </si>
+  <si>
+    <t>efficiency</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -211,6 +209,13 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -298,7 +303,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="117">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -416,8 +421,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -446,8 +453,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="117">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -506,6 +514,7 @@
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -564,6 +573,7 @@
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -593,6 +603,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000"/>
+              <a:t>Performance</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1000" baseline="0"/>
+              <a:t> of sum (10M) with different scheduling policy</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1000"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -659,28 +693,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>29.999970999999999</c:v>
+                  <c:v>29.999971</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.000136999999999</c:v>
+                  <c:v>31.000137</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.999970999999999</c:v>
+                  <c:v>29.999971</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.999898999999999</c:v>
+                  <c:v>30.999899</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.999898999999999</c:v>
+                  <c:v>30.999899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31.000129999999999</c:v>
+                  <c:v>31.00013</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.999898999999999</c:v>
+                  <c:v>30.999899</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30.999898999999999</c:v>
+                  <c:v>30.999899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -747,28 +781,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>16.000029999999999</c:v>
+                  <c:v>16.00003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.999960000000002</c:v>
+                  <c:v>16.99996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.000032000000001</c:v>
+                  <c:v>16.000032</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.000032000000001</c:v>
+                  <c:v>16.000032</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.000032000000001</c:v>
+                  <c:v>16.000032</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.000032000000001</c:v>
+                  <c:v>16.000032</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.999960000000002</c:v>
+                  <c:v>16.99996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.000032000000001</c:v>
+                  <c:v>16.000032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -835,28 +869,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>9.0000630000000008</c:v>
+                  <c:v>9.000063000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0000630000000008</c:v>
+                  <c:v>9.000063000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.9998249999999995</c:v>
+                  <c:v>8.999825</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0001350000000002</c:v>
+                  <c:v>8.000135</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0001350000000002</c:v>
+                  <c:v>8.000135</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.0000630000000008</c:v>
+                  <c:v>9.000063000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.9998969999999998</c:v>
+                  <c:v>7.999897</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.9998969999999998</c:v>
+                  <c:v>7.999897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -923,28 +957,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>5.0001139999999999</c:v>
+                  <c:v>5.000114</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0001139999999999</c:v>
+                  <c:v>5.000114</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0001139999999999</c:v>
+                  <c:v>5.000114</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9998760000000004</c:v>
+                  <c:v>4.999876</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0001139999999999</c:v>
+                  <c:v>5.000114</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0001139999999999</c:v>
+                  <c:v>5.000114</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0001139999999999</c:v>
+                  <c:v>5.000114</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9998699999999996</c:v>
+                  <c:v>4.99987</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1011,28 +1045,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>30.999898999999999</c:v>
+                  <c:v>30.999899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.999898999999999</c:v>
+                  <c:v>30.999899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.999970999999999</c:v>
+                  <c:v>29.999971</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.999970999999999</c:v>
+                  <c:v>29.999971</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32.000064999999999</c:v>
+                  <c:v>32.000065</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.000064999999999</c:v>
+                  <c:v>32.000065</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>37.000179000000003</c:v>
+                  <c:v>37.000179</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31.000129999999999</c:v>
+                  <c:v>31.00013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1099,28 +1133,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>14.999866000000001</c:v>
+                  <c:v>14.999866</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.000032000000001</c:v>
+                  <c:v>16.000032</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16.999960000000002</c:v>
+                  <c:v>16.99996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.999980999999998</c:v>
+                  <c:v>19.999981</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.000032000000001</c:v>
+                  <c:v>16.000032</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.999980999999998</c:v>
+                  <c:v>19.999981</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55.999994000000001</c:v>
+                  <c:v>55.999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.000032000000001</c:v>
+                  <c:v>16.000032</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1187,28 +1221,28 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7.9998969999999998</c:v>
+                  <c:v>7.999897</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.9998969999999998</c:v>
+                  <c:v>7.999897</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.9999900000000004</c:v>
+                  <c:v>9.99999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.999866000000001</c:v>
+                  <c:v>14.999866</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.9998969999999998</c:v>
+                  <c:v>7.999897</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.999917999999999</c:v>
+                  <c:v>10.999918</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>59.000014999999998</c:v>
+                  <c:v>59.000015</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0001350000000002</c:v>
+                  <c:v>8.000135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1278,25 +1312,25 @@
                   <c:v>3.999949</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9998760000000004</c:v>
+                  <c:v>4.999876</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.9999690000000001</c:v>
+                  <c:v>6.999969</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0001350000000002</c:v>
+                  <c:v>8.000135</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>3.999949</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.9998969999999998</c:v>
+                  <c:v>7.999897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>67.999840000000006</c:v>
+                  <c:v>67.99984</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0001139999999999</c:v>
+                  <c:v>5.000114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1313,11 +1347,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137662024"/>
-        <c:axId val="137662416"/>
+        <c:axId val="-2112732552"/>
+        <c:axId val="-2084638456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137662024"/>
+        <c:axId val="-2112732552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1327,7 +1361,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137662416"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2084638456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1335,18 +1379,47 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137662416"/>
+        <c:axId val="-2084638456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="800"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="800"/>
+                  <a:t>Execution Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137662024"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2112732552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1355,6 +1428,16 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="800"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1362,7 +1445,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1412,8 +1495,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12359011373578303"/>
-          <c:y val="2.7777777777777776E-2"/>
+          <c:x val="0.123590113735783"/>
+          <c:y val="0.0277777777777778"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1424,26 +1507,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1452,10 +1515,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14831006241135339"/>
-          <c:y val="0.17171296296296296"/>
-          <c:w val="0.82927044293619889"/>
-          <c:h val="0.62271617089530473"/>
+          <c:x val="0.148310062411353"/>
+          <c:y val="0.171712962962963"/>
+          <c:w val="0.829270442936199"/>
+          <c:h val="0.622716170895305"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1498,16 +1561,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1519,16 +1582,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>31.000012699999999</c:v>
+                  <c:v>31.0000127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.999867999999999</c:v>
+                  <c:v>14.999868</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0001350000000002</c:v>
+                  <c:v>8.000135</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.9994900000000002</c:v>
+                  <c:v>3.99949</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1567,21 +1630,6 @@
           </c:marker>
           <c:dPt>
             <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
           <c:cat>
@@ -1591,16 +1639,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1612,13 +1660,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>29.999970999999999</c:v>
+                  <c:v>29.999971</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.000032000000001</c:v>
+                  <c:v>16.000032</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.9999897000000004</c:v>
+                  <c:v>7.9999897</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5.0000114</c:v>
@@ -1638,11 +1686,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="222769752"/>
-        <c:axId val="223284968"/>
+        <c:axId val="-2127000120"/>
+        <c:axId val="-2111944712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222769752"/>
+        <c:axId val="-2127000120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1683,26 +1731,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1741,7 +1769,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223284968"/>
+        <c:crossAx val="-2111944712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1749,7 +1777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="223284968"/>
+        <c:axId val="-2111944712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1809,26 +1837,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1861,7 +1869,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222769752"/>
+        <c:crossAx val="-2127000120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="2.5"/>
@@ -1880,10 +1888,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.65424194646174272"/>
-          <c:y val="0.22763815981335667"/>
-          <c:w val="0.29547102175643875"/>
-          <c:h val="0.15625109361329836"/>
+          <c:x val="0.654241946461743"/>
+          <c:y val="0.227638159813357"/>
+          <c:w val="0.295471021756439"/>
+          <c:h val="0.156251093613298"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2001,8 +2009,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12359011373578303"/>
-          <c:y val="2.7777777777777776E-2"/>
+          <c:x val="0.123590113735783"/>
+          <c:y val="0.0277777777777778"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2013,26 +2021,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2077,16 +2065,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9331</c:v>
+                  <c:v>9331.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4677</c:v>
+                  <c:v>4677.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2421</c:v>
+                  <c:v>2421.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1252</c:v>
+                  <c:v>1252.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2134,10 +2122,10 @@
                   <c:v>4713.99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2454.9899999999998</c:v>
+                  <c:v>2454.99</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1265</c:v>
+                  <c:v>1265.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2176,21 +2164,6 @@
           </c:marker>
           <c:dPt>
             <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="triangle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
           <c:cat>
@@ -2200,16 +2173,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2227,7 +2200,7 @@
                   <c:v>4722.99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2431.9899999999998</c:v>
+                  <c:v>2431.99</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1269.99</c:v>
@@ -2274,16 +2247,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9324</c:v>
+                  <c:v>9324.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4700</c:v>
+                  <c:v>4700.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2404</c:v>
+                  <c:v>2404.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1259</c:v>
+                  <c:v>1259.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2328,10 +2301,10 @@
                   <c:v>9322.99</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4687</c:v>
+                  <c:v>4687.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2365</c:v>
+                  <c:v>2365.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1271.99</c:v>
@@ -2378,16 +2351,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2399,16 +2372,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9325</c:v>
+                  <c:v>9325.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4680</c:v>
+                  <c:v>4680.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2377</c:v>
+                  <c:v>2377.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1262</c:v>
+                  <c:v>1262.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2425,11 +2398,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="467347216"/>
-        <c:axId val="467351136"/>
+        <c:axId val="-2084700936"/>
+        <c:axId val="-2119112616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="467347216"/>
+        <c:axId val="-2084700936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2470,26 +2443,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2528,7 +2481,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467351136"/>
+        <c:crossAx val="-2119112616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2536,7 +2489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="467351136"/>
+        <c:axId val="-2119112616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2596,26 +2549,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2648,7 +2581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="467347216"/>
+        <c:crossAx val="-2084700936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2778,8 +2711,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.26255504607043834"/>
-          <c:y val="4.6296296296296294E-2"/>
+          <c:x val="0.262555046070438"/>
+          <c:y val="0.0462962962962963"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2790,26 +2723,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2818,10 +2731,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14788528032580517"/>
-          <c:y val="0.17171296296296296"/>
-          <c:w val="0.81088026532290425"/>
-          <c:h val="0.62271617089530473"/>
+          <c:x val="0.147885280325805"/>
+          <c:y val="0.171712962962963"/>
+          <c:w val="0.810880265322904"/>
+          <c:h val="0.622716170895305"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2859,21 +2772,6 @@
           </c:marker>
           <c:dPt>
             <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="circle"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
           <c:cat>
@@ -2883,16 +2781,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2904,16 +2802,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8749944375111247</c:v>
+                  <c:v>1.874994437511125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.7500012031265486</c:v>
+                  <c:v>3.750001203126549</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9999805200444136</c:v>
+                  <c:v>5.999980520044414</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2957,16 +2855,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2978,16 +2876,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.96774060353852687</c:v>
+                  <c:v>0.967740603538527</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0000156668045346</c:v>
+                  <c:v>2.000015666804535</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.7499330948790237</c:v>
+                  <c:v>3.749933094879024</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.500949121012928</c:v>
+                  <c:v>7.500949121012927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3004,11 +2902,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="474585976"/>
-        <c:axId val="474588328"/>
+        <c:axId val="-2085610984"/>
+        <c:axId val="-2084615768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="474585976"/>
+        <c:axId val="-2085610984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3049,26 +2947,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3107,7 +2985,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474588328"/>
+        <c:crossAx val="-2084615768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3115,7 +2993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="474588328"/>
+        <c:axId val="-2084615768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3170,26 +3048,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3222,10 +3080,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474585976"/>
+        <c:crossAx val="-2085610984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1"/>
+        <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3241,10 +3099,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.62169806343781175"/>
-          <c:y val="0.6257863079615047"/>
-          <c:w val="0.33827935387909552"/>
-          <c:h val="0.15625109361329834"/>
+          <c:x val="0.621698063437812"/>
+          <c:y val="0.625786307961505"/>
+          <c:w val="0.338279353879096"/>
+          <c:h val="0.156251093613298"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3362,8 +3220,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12359011373578303"/>
-          <c:y val="2.7777777777777776E-2"/>
+          <c:x val="0.123590113735783"/>
+          <c:y val="0.0277777777777778"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3374,26 +3232,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3438,16 +3276,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9950823177250374</c:v>
+                  <c:v>1.995082317725037</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8541924824452707</c:v>
+                  <c:v>3.854192482445271</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.4528753993610222</c:v>
+                  <c:v>7.452875399361022</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3491,16 +3329,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.99139501848174516</c:v>
+                  <c:v>0.991395018481745</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9794271943724955</c:v>
+                  <c:v>1.979427194372495</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8008301459476415</c:v>
+                  <c:v>3.800830145947641</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.3762845849802368</c:v>
+                  <c:v>7.376284584980236</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3539,21 +3377,6 @@
           </c:marker>
           <c:dPt>
             <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="x"/>
-              <c:size val="5"/>
-              <c:spPr>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="accent1"/>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
           <c:cat>
@@ -3563,16 +3386,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3584,16 +3407,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.99171111883422136</c:v>
+                  <c:v>0.991711118834221</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9756552522872164</c:v>
+                  <c:v>1.975655252287216</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8367756446366972</c:v>
+                  <c:v>3.836775644636697</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.3473019472594272</c:v>
+                  <c:v>7.347301947259427</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3637,16 +3460,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0007507507507507</c:v>
+                  <c:v>1.000750750750751</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9853191489361701</c:v>
+                  <c:v>1.98531914893617</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8814475873544092</c:v>
+                  <c:v>3.881447587354409</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.4114376489277207</c:v>
+                  <c:v>7.411437648927721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3690,16 +3513,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0008591664262216</c:v>
+                  <c:v>1.000859166426222</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9908256880733946</c:v>
+                  <c:v>1.990825688073395</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9454545454545453</c:v>
+                  <c:v>3.945454545454545</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.3357494948859658</c:v>
+                  <c:v>7.335749494885965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3743,16 +3566,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3764,16 +3587,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0006434316353887</c:v>
+                  <c:v>1.000643431635389</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9938034188034188</c:v>
+                  <c:v>1.993803418803419</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9255363904080776</c:v>
+                  <c:v>3.925536390408078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.3938193343898577</c:v>
+                  <c:v>7.393819334389858</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3790,11 +3613,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="474571080"/>
-        <c:axId val="474567552"/>
+        <c:axId val="-2108425704"/>
+        <c:axId val="-2083590536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="474571080"/>
+        <c:axId val="-2108425704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3835,26 +3658,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -3893,7 +3696,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474567552"/>
+        <c:crossAx val="-2083590536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3901,7 +3704,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="474567552"/>
+        <c:axId val="-2083590536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3956,26 +3759,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -4008,7 +3791,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="474571080"/>
+        <c:crossAx val="-2108425704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6347,16 +6130,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>331304</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>788504</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>149087</xdr:rowOff>
+      <xdr:rowOff>138927</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>72887</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>530087</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>109331</xdr:rowOff>
+      <xdr:rowOff>99171</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6377,16 +6160,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>238538</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>462058</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>125895</xdr:rowOff>
+      <xdr:rowOff>85255</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>298174</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>521694</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>86139</xdr:rowOff>
+      <xdr:rowOff>45499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6798,315 +6581,545 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="48.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="D3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="D4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="D5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="D6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="D7">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C13" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1">
         <v>29.999970999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C14" s="12">
+        <f>$B$14/(B14*D14)</f>
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="1">
         <v>16.000032000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" s="12">
+        <f>$B$14/(B15*D15)</f>
+        <v>0.93749721875556236</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="1">
         <v>7.9999897000000004</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="12">
+        <f t="shared" ref="C16:C21" si="0">$B$14/(B16*D16)</f>
+        <v>0.93750030078163715</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="2">
         <v>5.0000114</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="12">
+        <f t="shared" si="0"/>
+        <v>0.7499975650055517</v>
+      </c>
+      <c r="D17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="1">
         <v>31.000012699999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="12">
+        <f t="shared" si="0"/>
+        <v>0.96774060353852687</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B19" s="1">
         <v>14.999867999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="12">
+        <f t="shared" si="0"/>
+        <v>1.0000078334022673</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="1">
         <v>8.0001350000000002</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="12">
+        <f t="shared" si="0"/>
+        <v>0.93748327371975593</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="2">
         <v>3.9994900000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="12">
+        <f t="shared" si="0"/>
+        <v>0.937618640126616</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="8"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="1">
         <v>9331</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="12">
+        <f>$B$27/(B27*D27)</f>
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B28" s="1">
         <v>4677</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" s="12">
+        <f t="shared" ref="C28:C50" si="1">$B$27/(B28*D28)</f>
+        <v>0.99754115886251871</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B29" s="1">
         <v>2421</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" s="12">
+        <f t="shared" si="1"/>
+        <v>0.96354812061131767</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="2">
         <v>1252</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" s="12">
+        <f t="shared" si="1"/>
+        <v>0.93160942492012777</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="1">
         <v>9411.99</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" s="12">
+        <f t="shared" si="1"/>
+        <v>0.99139501848174516</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B32" s="1">
         <v>4713.99</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="12">
+        <f t="shared" si="1"/>
+        <v>0.98971359718624774</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B33" s="1">
         <v>2454.9899999999998</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" s="12">
+        <f t="shared" si="1"/>
+        <v>0.95020753648691036</v>
+      </c>
+      <c r="D33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="2">
         <v>1265</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" s="12">
+        <f t="shared" si="1"/>
+        <v>0.92203557312252959</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="1">
         <v>9408.99</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" s="12">
+        <f t="shared" si="1"/>
+        <v>0.99171111883422136</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B36" s="1">
         <v>4722.99</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9878276261436082</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B37" s="1">
         <v>2431.9899999999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9591939111591743</v>
+      </c>
+      <c r="D37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="2">
         <v>1269.99</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9184127434074284</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B39" s="1">
         <v>9324</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0007507507507507</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B40" s="1">
         <v>4700</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40" s="12">
+        <f t="shared" si="1"/>
+        <v>0.99265957446808506</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="1">
         <v>2404</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41" s="12">
+        <f t="shared" si="1"/>
+        <v>0.9703618968386023</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B42" s="2">
         <v>1259</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42" s="12">
+        <f t="shared" si="1"/>
+        <v>0.92642970611596509</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B43" s="1">
         <v>9322.99</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0008591664262216</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B44" s="1">
         <v>4687</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44" s="12">
+        <f t="shared" si="1"/>
+        <v>0.99541284403669728</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B45" s="1">
         <v>2365</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45" s="12">
+        <f t="shared" si="1"/>
+        <v>0.98636363636363633</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B46" s="2">
         <v>1271.99</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46" s="12">
+        <f t="shared" si="1"/>
+        <v>0.91696868686074573</v>
+      </c>
+      <c r="D46">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B47" s="1">
         <v>9325</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0006434316353887</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B48" s="1">
         <v>4680</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48" s="12">
+        <f t="shared" si="1"/>
+        <v>0.99690170940170941</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B49" s="1">
         <v>2377</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49" s="12">
+        <f t="shared" si="1"/>
+        <v>0.98138409760201939</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B50" s="2">
         <v>1262</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50" s="12">
+        <f t="shared" si="1"/>
+        <v>0.92422741679873222</v>
+      </c>
+      <c r="D50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B56" s="8"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4">
       <c r="A57" s="3" t="s">
         <v>0</v>
       </c>
@@ -7115,7 +7128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4">
       <c r="A58" s="3" t="s">
         <v>2</v>
       </c>
@@ -7124,7 +7137,7 @@
         <v>1.8749944375111247</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4">
       <c r="A59" s="3" t="s">
         <v>4</v>
       </c>
@@ -7133,7 +7146,7 @@
         <v>3.7500012031265486</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4">
       <c r="A60" s="3" t="s">
         <v>6</v>
       </c>
@@ -7142,7 +7155,7 @@
         <v>5.9999805200444136</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4">
       <c r="A61" s="3" t="s">
         <v>1</v>
       </c>
@@ -7151,7 +7164,7 @@
         <v>0.96774060353852687</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4">
       <c r="A62" s="3" t="s">
         <v>3</v>
       </c>
@@ -7160,7 +7173,7 @@
         <v>2.0000156668045346</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4">
       <c r="A63" s="3" t="s">
         <v>5</v>
       </c>
@@ -7169,7 +7182,7 @@
         <v>3.7499330948790237</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4">
       <c r="A64" s="3" t="s">
         <v>7</v>
       </c>
@@ -7178,13 +7191,13 @@
         <v>7.500949121012928</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2">
       <c r="A70" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B70" s="8"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2">
       <c r="A71" s="3" t="s">
         <v>8</v>
       </c>
@@ -7193,7 +7206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2">
       <c r="A72" s="3" t="s">
         <v>9</v>
       </c>
@@ -7202,7 +7215,7 @@
         <v>1.9950823177250374</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2">
       <c r="A73" s="3" t="s">
         <v>10</v>
       </c>
@@ -7211,7 +7224,7 @@
         <v>3.8541924824452707</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2">
       <c r="A74" s="3" t="s">
         <v>11</v>
       </c>
@@ -7220,7 +7233,7 @@
         <v>7.4528753993610222</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2">
       <c r="A75" s="3" t="s">
         <v>12</v>
       </c>
@@ -7229,7 +7242,7 @@
         <v>0.99139501848174516</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2">
       <c r="A76" s="3" t="s">
         <v>13</v>
       </c>
@@ -7238,7 +7251,7 @@
         <v>1.9794271943724955</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2">
       <c r="A77" s="3" t="s">
         <v>14</v>
       </c>
@@ -7247,7 +7260,7 @@
         <v>3.8008301459476415</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2">
       <c r="A78" s="3" t="s">
         <v>15</v>
       </c>
@@ -7256,7 +7269,7 @@
         <v>7.3762845849802368</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2">
       <c r="A79" s="3" t="s">
         <v>16</v>
       </c>
@@ -7265,7 +7278,7 @@
         <v>0.99171111883422136</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2">
       <c r="A80" s="3" t="s">
         <v>17</v>
       </c>
@@ -7274,7 +7287,7 @@
         <v>1.9756552522872164</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2">
       <c r="A81" s="3" t="s">
         <v>18</v>
       </c>
@@ -7283,7 +7296,7 @@
         <v>3.8367756446366972</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2">
       <c r="A82" s="3" t="s">
         <v>19</v>
       </c>
@@ -7292,7 +7305,7 @@
         <v>7.3473019472594272</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2">
       <c r="A83" s="3" t="s">
         <v>20</v>
       </c>
@@ -7301,7 +7314,7 @@
         <v>1.0007507507507507</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2">
       <c r="A84" s="3" t="s">
         <v>21</v>
       </c>
@@ -7310,7 +7323,7 @@
         <v>1.9853191489361701</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2">
       <c r="A85" s="3" t="s">
         <v>22</v>
       </c>
@@ -7319,7 +7332,7 @@
         <v>3.8814475873544092</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2">
       <c r="A86" s="3" t="s">
         <v>23</v>
       </c>
@@ -7328,7 +7341,7 @@
         <v>7.4114376489277207</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2">
       <c r="A87" s="3" t="s">
         <v>24</v>
       </c>
@@ -7337,7 +7350,7 @@
         <v>1.0008591664262216</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2">
       <c r="A88" s="3" t="s">
         <v>25</v>
       </c>
@@ -7346,7 +7359,7 @@
         <v>1.9908256880733946</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2">
       <c r="A89" s="3" t="s">
         <v>26</v>
       </c>
@@ -7355,7 +7368,7 @@
         <v>3.9454545454545453</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2">
       <c r="A90" s="3" t="s">
         <v>27</v>
       </c>
@@ -7364,7 +7377,7 @@
         <v>7.3357494948859658</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2">
       <c r="A91" s="3" t="s">
         <v>28</v>
       </c>
@@ -7373,7 +7386,7 @@
         <v>1.0006434316353887</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2">
       <c r="A92" s="3" t="s">
         <v>29</v>
       </c>
@@ -7382,7 +7395,7 @@
         <v>1.9938034188034188</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2">
       <c r="A93" s="3" t="s">
         <v>30</v>
       </c>
@@ -7391,7 +7404,7 @@
         <v>3.9255363904080776</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2">
       <c r="A94" s="3" t="s">
         <v>31</v>
       </c>
@@ -7400,13 +7413,13 @@
         <v>7.3938193343898577</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9">
       <c r="A100" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B100" s="10"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9">
       <c r="A101" s="6"/>
       <c r="B101" s="11" t="s">
         <v>44</v>
@@ -7419,7 +7432,7 @@
       <c r="H101" s="11"/>
       <c r="I101" s="11"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9">
       <c r="A102" s="6"/>
       <c r="B102" s="7" t="s">
         <v>36</v>
@@ -7446,7 +7459,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9">
       <c r="A103" s="3" t="s">
         <v>0</v>
       </c>
@@ -7475,7 +7488,7 @@
         <v>30.999898999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9">
       <c r="A104" s="3" t="s">
         <v>2</v>
       </c>
@@ -7504,7 +7517,7 @@
         <v>16.000032000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9">
       <c r="A105" s="3" t="s">
         <v>4</v>
       </c>
@@ -7533,7 +7546,7 @@
         <v>7.9998969999999998</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9">
       <c r="A106" s="3" t="s">
         <v>6</v>
       </c>
@@ -7562,7 +7575,7 @@
         <v>4.9998699999999996</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9">
       <c r="A107" s="3" t="s">
         <v>1</v>
       </c>
@@ -7591,7 +7604,7 @@
         <v>31.000129999999999</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9">
       <c r="A108" s="3" t="s">
         <v>3</v>
       </c>
@@ -7620,7 +7633,7 @@
         <v>16.000032000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9">
       <c r="A109" s="3" t="s">
         <v>5</v>
       </c>
@@ -7649,7 +7662,7 @@
         <v>8.0001350000000002</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9">
       <c r="A110" s="3" t="s">
         <v>7</v>
       </c>
@@ -7678,7 +7691,7 @@
         <v>5.0001139999999999</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2">
       <c r="B126" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on assignment 2 report.
</commit_message>
<xml_diff>
--- a/Assignment2/Report/Assignment_2_result_plot_Kazumi_v2.xlsx
+++ b/Assignment2/Report/Assignment_2_result_plot_Kazumi_v2.xlsx
@@ -224,12 +224,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="6">
@@ -306,7 +312,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="119">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -426,8 +432,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -457,8 +467,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="119">
+  <cellStyles count="123">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -518,6 +529,8 @@
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -577,6 +590,8 @@
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6163,16 +6178,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>655098</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>756698</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>85255</xdr:rowOff>
+      <xdr:rowOff>115735</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>714734</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>816334</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>45499</xdr:rowOff>
+      <xdr:rowOff>75979</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6584,8 +6599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6687,7 +6702,7 @@
         <v>1.9999878000000031</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:7">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
@@ -6706,7 +6721,7 @@
         <v>10.000120200000001</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
@@ -6725,7 +6740,7 @@
         <v>1.0000417000000006</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:7">
       <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
@@ -6744,7 +6759,7 @@
         <v>-2.3499999999998522E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -6763,7 +6778,7 @@
         <v>2.0005690000000023</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:7">
       <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
@@ -6782,7 +6797,12 @@
         <v>1.9959490000000031</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="25" spans="1:7">
+      <c r="G25">
+        <v>6865</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="9" t="s">
         <v>33</v>
       </c>
@@ -6791,11 +6811,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="13">
         <v>9331</v>
       </c>
       <c r="C27" s="8">
@@ -6809,8 +6829,12 @@
         <f>B27*D27-$B$27</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <f>B27/$G$25</f>
+        <v>1.3592134013109978</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="3" t="s">
         <v>9</v>
       </c>
@@ -6829,7 +6853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:7">
       <c r="A29" s="3" t="s">
         <v>10</v>
       </c>
@@ -6848,7 +6872,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:7">
       <c r="A30" s="3" t="s">
         <v>11</v>
       </c>
@@ -6867,11 +6891,11 @@
         <v>685</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:7">
       <c r="A31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="13">
         <v>9411.99</v>
       </c>
       <c r="C31" s="8">
@@ -6885,8 +6909,12 @@
         <f t="shared" si="3"/>
         <v>80.989999999999782</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31">
+        <f>B31/$G$25</f>
+        <v>1.3710109249817917</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="3" t="s">
         <v>13</v>
       </c>
@@ -6905,7 +6933,7 @@
         <v>96.979999999999563</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
         <v>14</v>
       </c>
@@ -6924,7 +6952,7 @@
         <v>488.95999999999913</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
         <v>15</v>
       </c>
@@ -6943,11 +6971,11 @@
         <v>789</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:8">
       <c r="A35" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="13">
         <v>9408.99</v>
       </c>
       <c r="C35" s="8">
@@ -6961,8 +6989,12 @@
         <f t="shared" si="3"/>
         <v>77.989999999999782</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35">
+        <f>B35/$G$25</f>
+        <v>1.3705739257101237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
         <v>17</v>
       </c>
@@ -6981,7 +7013,7 @@
         <v>114.97999999999956</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
@@ -7000,7 +7032,7 @@
         <v>396.95999999999913</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:8">
       <c r="A38" s="3" t="s">
         <v>19</v>
       </c>
@@ -7019,11 +7051,11 @@
         <v>828.92000000000007</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="13">
         <v>9324</v>
       </c>
       <c r="C39" s="8">
@@ -7037,8 +7069,12 @@
         <f t="shared" si="3"/>
         <v>-7</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39">
+        <f>B39/$G$25</f>
+        <v>1.3581937363437728</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="3" t="s">
         <v>21</v>
       </c>
@@ -7057,7 +7093,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:8">
       <c r="A41" s="3" t="s">
         <v>22</v>
       </c>
@@ -7076,7 +7112,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
         <v>23</v>
       </c>
@@ -7095,11 +7131,11 @@
         <v>741</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="13">
         <v>9322.99</v>
       </c>
       <c r="C43" s="8">
@@ -7113,8 +7149,12 @@
         <f t="shared" si="3"/>
         <v>-8.0100000000002183</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43">
+        <f>B43/$G$25</f>
+        <v>1.3580466132556446</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="3" t="s">
         <v>25</v>
       </c>
@@ -7133,7 +7173,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:8">
       <c r="A45" s="3" t="s">
         <v>26</v>
       </c>
@@ -7152,7 +7192,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:8">
       <c r="A46" s="3" t="s">
         <v>27</v>
       </c>
@@ -7171,11 +7211,11 @@
         <v>844.92000000000007</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:8">
       <c r="A47" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="13">
         <v>9325</v>
       </c>
       <c r="C47" s="8">
@@ -7189,8 +7229,12 @@
         <f t="shared" si="3"/>
         <v>-6</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47">
+        <f>B47/$G$25</f>
+        <v>1.3583394027676621</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="3" t="s">
         <v>29</v>
       </c>
@@ -7208,6 +7252,10 @@
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
+      <c r="H48">
+        <f>B32/B28</f>
+        <v>1.0079089159717767</v>
+      </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3" t="s">
@@ -7245,6 +7293,12 @@
       <c r="E50">
         <f t="shared" si="3"/>
         <v>765</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="B52">
+        <f>B50/B27</f>
+        <v>0.1352480977387204</v>
       </c>
     </row>
     <row r="56" spans="1:5">

</xml_diff>